<commit_message>
redo v1, no rate limit closed loop
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/tr_header.xlsx
+++ b/myESC-Particle-DEV/saves/tr_header.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\ESC\myESC-Particle-DEV\saves\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19656" windowHeight="8388"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19650" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="tr_header" sheetId="1" r:id="rId1"/>
@@ -850,7 +845,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -862,15 +857,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>